<commit_message>
added gradientbooster.py which optimizes a model from a given list of parameters and range
</commit_message>
<xml_diff>
--- a/Data/combined_data.xlsx
+++ b/Data/combined_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\PycharmProjects\Aeroacoustic_Prediction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9677C27B-EE55-4558-9775-20C87975FA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E466CE26-D726-46EC-9D28-0CA968551006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A23546F3-748E-4109-9CA5-4CA9C3EFA839}"/>
   </bookViews>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A04D9-5AFF-47BC-A671-2EB6D72E5E00}">
   <dimension ref="A1:F553"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="64" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,11 +737,11 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D34" si="2">1065*COS(RADIANS(B15-10))</f>
+        <f t="shared" ref="D15:D24" si="2">1065*COS(RADIANS(B15-10))</f>
         <v>-184.93530921528077</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:E34" si="3">1065*SIN(RADIANS(B15-10))</f>
+        <f t="shared" ref="E15:E24" si="3">1065*SIN(RADIANS(B15-10))</f>
         <v>1048.8202569580014</v>
       </c>
       <c r="F15">
@@ -6241,7 +6241,7 @@
         <v>-184.93530921528077</v>
       </c>
       <c r="E268" s="2">
-        <f t="shared" ref="E268:E287" si="25">1065*SIN(RADIANS(B268-10))</f>
+        <f t="shared" ref="E268:E277" si="25">1065*SIN(RADIANS(B268-10))</f>
         <v>1048.8202569580014</v>
       </c>
       <c r="F268">

</xml_diff>